<commit_message>
Daily push for 20200520
</commit_message>
<xml_diff>
--- a/Graphics/20200520/20200520_Kosovo_COVID.xlsx
+++ b/Graphics/20200520/20200520_Kosovo_COVID.xlsx
@@ -494,43 +494,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>245.5</v>
+        <v>245.5714285714286</v>
       </c>
       <c r="C3" t="n">
         <v>9.5</v>
       </c>
       <c r="D3" t="n">
-        <v>18.85714285714286</v>
+        <v>19.92857142857143</v>
       </c>
       <c r="E3" t="n">
-        <v>1.142857142857143</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="F3" t="n">
-        <v>10609.28571428571</v>
+        <v>10602.92857142857</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0436829109177748</v>
+        <v>0.04356462792655074</v>
       </c>
       <c r="H3" t="n">
-        <v>905.7142857142857</v>
+        <v>922.7142857142857</v>
       </c>
       <c r="I3" t="n">
         <v>0.7480481388866485</v>
       </c>
       <c r="J3" t="n">
-        <v>3.787017210023278</v>
+        <v>3.784982313396027</v>
       </c>
       <c r="K3" t="n">
-        <v>675.7142857142857</v>
+        <v>669.7142857142857</v>
       </c>
       <c r="L3" t="n">
-        <v>1.722605373071447</v>
+        <v>1.686480578325963</v>
       </c>
       <c r="M3" t="n">
-        <v>34.5</v>
+        <v>28.35714285714286</v>
       </c>
       <c r="N3" t="n">
-        <v>0.09523809523809522</v>
+        <v>-0.1428571428571428</v>
       </c>
     </row>
     <row r="4">
@@ -540,22 +540,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>62.12363603207843</v>
+        <v>62.06288905458879</v>
       </c>
       <c r="C4" t="n">
         <v>7.783117824941563</v>
       </c>
       <c r="D4" t="n">
-        <v>16.17147128484244</v>
+        <v>17.28255806259054</v>
       </c>
       <c r="E4" t="n">
-        <v>1.350620533005412</v>
+        <v>0.4258153136263202</v>
       </c>
       <c r="F4" t="n">
-        <v>1030.525364788527</v>
+        <v>1030.92829447622</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3202075714990438</v>
+        <v>0.3197112084771773</v>
       </c>
       <c r="H4" t="n">
         <v>50.86698879873419</v>
@@ -564,19 +564,19 @@
         <v>2.110102634057612</v>
       </c>
       <c r="J4" t="n">
-        <v>2.765891900922463</v>
+        <v>2.764455872658345</v>
       </c>
       <c r="K4" t="n">
         <v>66.52984127607536</v>
       </c>
       <c r="L4" t="n">
-        <v>5.81813582719399</v>
+        <v>5.831209625978868</v>
       </c>
       <c r="M4" t="n">
-        <v>5.626175090933995</v>
+        <v>0.9287827316640653</v>
       </c>
       <c r="N4" t="n">
-        <v>1.049448951280195</v>
+        <v>0.3631365196012815</v>
       </c>
     </row>
     <row r="5">
@@ -598,13 +598,13 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>9090</v>
+        <v>9083</v>
       </c>
       <c r="G5" t="n">
         <v>-0.5036855036855037</v>
       </c>
       <c r="H5" t="n">
-        <v>843</v>
+        <v>860</v>
       </c>
       <c r="I5" t="n">
         <v>-0.75</v>
@@ -613,7 +613,7 @@
         <v>0.411522633744856</v>
       </c>
       <c r="K5" t="n">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="L5" t="n">
         <v>-1</v>
@@ -644,13 +644,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>9789</v>
+        <v>9782</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.165</v>
+        <v>-0.16375</v>
       </c>
       <c r="H6" t="n">
-        <v>856.5</v>
+        <v>873.5</v>
       </c>
       <c r="I6" t="n">
         <v>-0.6428571428571428</v>
@@ -659,16 +659,16 @@
         <v>1.300925925925926</v>
       </c>
       <c r="K6" t="n">
-        <v>659.5</v>
+        <v>653.5</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.4560617613419748</v>
+        <v>-0.5022611644997174</v>
       </c>
       <c r="M6" t="n">
-        <v>30.25</v>
+        <v>28</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.9166666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -687,16 +687,16 @@
         <v>18.5</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10519.5</v>
+        <v>10513.5</v>
       </c>
       <c r="G7" t="n">
         <v>0.0236089494163424</v>
       </c>
       <c r="H7" t="n">
-        <v>906</v>
+        <v>923</v>
       </c>
       <c r="I7" t="n">
         <v>-0.1071428571428572</v>
@@ -705,13 +705,13 @@
         <v>3.851317335123343</v>
       </c>
       <c r="K7" t="n">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.08333333333333331</v>
+        <v>-0.1920289855072463</v>
       </c>
       <c r="M7" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -733,34 +733,34 @@
         <v>26.75</v>
       </c>
       <c r="E8" t="n">
-        <v>1.75</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>11488.25</v>
+        <v>11482.25</v>
       </c>
       <c r="G8" t="n">
         <v>0.1648388168826853</v>
       </c>
       <c r="H8" t="n">
-        <v>955.25</v>
+        <v>972.25</v>
       </c>
       <c r="I8" t="n">
         <v>1.232954545454545</v>
       </c>
       <c r="J8" t="n">
-        <v>5.641390462819034</v>
+        <v>5.634268324623655</v>
       </c>
       <c r="K8" t="n">
-        <v>713.5</v>
+        <v>707.5</v>
       </c>
       <c r="L8" t="n">
         <v>0.03409090909090906</v>
       </c>
       <c r="M8" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="N8" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -779,16 +779,16 @@
         <v>61</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>12203</v>
+        <v>12197</v>
       </c>
       <c r="G9" t="n">
         <v>0.7245762711864407</v>
       </c>
       <c r="H9" t="n">
-        <v>972</v>
+        <v>989</v>
       </c>
       <c r="I9" t="n">
         <v>7</v>
@@ -797,16 +797,16 @@
         <v>9.338521400778211</v>
       </c>
       <c r="K9" t="n">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="L9" t="n">
         <v>21</v>
       </c>
       <c r="M9" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="N9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -948,43 +948,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>145.2738095238095</v>
+        <v>145.202380952381</v>
       </c>
       <c r="C3" t="n">
-        <v>11.57142857142857</v>
+        <v>11.77380952380952</v>
       </c>
       <c r="D3" t="n">
-        <v>9.226190476190476</v>
+        <v>9.154761904761905</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5</v>
+        <v>0.3452380952380952</v>
       </c>
       <c r="F3" t="n">
-        <v>3874.297619047619</v>
+        <v>3871.595238095238</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3563069029016233</v>
+        <v>0.3662432723157148</v>
       </c>
       <c r="H3" t="n">
-        <v>371.5357142857143</v>
+        <v>374.9761904761905</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6429610775126213</v>
+        <v>0.6605708486938211</v>
       </c>
       <c r="J3" t="n">
-        <v>7.265431440600751</v>
+        <v>7.317510264686279</v>
       </c>
       <c r="K3" t="n">
-        <v>171.3928571428571</v>
+        <v>169.3690476190476</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9232367310256466</v>
+        <v>0.9412141240030396</v>
       </c>
       <c r="M3" t="n">
-        <v>11.30952380952381</v>
+        <v>10.26190476190476</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.07936507936507937</v>
+        <v>-0.1349206349206349</v>
       </c>
     </row>
     <row r="4">
@@ -994,43 +994,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>110.0367245585661</v>
+        <v>109.9938420797618</v>
       </c>
       <c r="C4" t="n">
-        <v>14.27043933796192</v>
+        <v>14.38234459033328</v>
       </c>
       <c r="D4" t="n">
-        <v>15.35786066181941</v>
+        <v>15.28326437061617</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9248900944150001</v>
+        <v>0.7196727438845412</v>
       </c>
       <c r="F4" t="n">
-        <v>3932.3438878771</v>
+        <v>3930.157316570051</v>
       </c>
       <c r="G4" t="n">
-        <v>1.345133734795482</v>
+        <v>1.350534704742466</v>
       </c>
       <c r="H4" t="n">
-        <v>366.3312230402734</v>
+        <v>371.3236816238768</v>
       </c>
       <c r="I4" t="n">
-        <v>2.131341288565056</v>
+        <v>2.135947705410573</v>
       </c>
       <c r="J4" t="n">
-        <v>7.669092421895789</v>
+        <v>7.65604245748536</v>
       </c>
       <c r="K4" t="n">
-        <v>251.6667340126737</v>
+        <v>248.469473035235</v>
       </c>
       <c r="L4" t="n">
-        <v>4.634771367467514</v>
+        <v>4.641660121019395</v>
       </c>
       <c r="M4" t="n">
-        <v>13.28100028029551</v>
+        <v>11.34573753369923</v>
       </c>
       <c r="N4" t="n">
-        <v>0.5311427089712333</v>
+        <v>0.3617192607698794</v>
       </c>
     </row>
     <row r="5">
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
         <v>-0.9333333333333333</v>
@@ -1098,10 +1098,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>310.25</v>
+        <v>309.25</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.2197643097643098</v>
+        <v>-0.2206060606060606</v>
       </c>
       <c r="H6" t="n">
         <v>19.75</v>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.1273809523809524</v>
+        <v>-0.175</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="G7" t="n">
         <v>0.06154113691695329</v>
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>4.593220338983051</v>
+        <v>4.714285714285714</v>
       </c>
       <c r="K7" t="n">
         <v>33.5</v>
@@ -1178,19 +1178,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>232.25</v>
+        <v>231.5</v>
       </c>
       <c r="C8" t="n">
-        <v>17.25</v>
+        <v>18.25</v>
       </c>
       <c r="D8" t="n">
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>7016.25</v>
+        <v>7011.25</v>
       </c>
       <c r="G8" t="n">
         <v>0.5428571428571429</v>
@@ -1199,7 +1199,7 @@
         <v>792.25</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7124999999999999</v>
+        <v>0.78125</v>
       </c>
       <c r="J8" t="n">
         <v>11.67064662639884</v>
@@ -1233,16 +1233,16 @@
         <v>87</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>12203</v>
+        <v>12197</v>
       </c>
       <c r="G9" t="n">
         <v>10.3</v>
       </c>
       <c r="H9" t="n">
-        <v>972</v>
+        <v>989</v>
       </c>
       <c r="I9" t="n">
         <v>13</v>
@@ -1251,16 +1251,16 @@
         <v>31.6</v>
       </c>
       <c r="K9" t="n">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="L9" t="n">
         <v>34</v>
       </c>
       <c r="M9" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="N9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1359,10 +1359,10 @@
         <v>43883</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1406,10 +1406,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6666666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
         <v>-0.4</v>
@@ -1494,7 +1494,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -1538,7 +1538,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
         <v>0.1666666666666667</v>
@@ -1582,7 +1582,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="n">
         <v>0.1428571428571428</v>
@@ -1626,7 +1626,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="n">
         <v>-0.75</v>
@@ -1670,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -1714,7 +1714,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" t="n">
         <v>0.75</v>
@@ -1758,7 +1758,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="n">
         <v>0.1428571428571428</v>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" t="n">
         <v>-0.875</v>
@@ -1846,7 +1846,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
@@ -1890,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" t="n">
         <v>0.25</v>
@@ -1934,7 +1934,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="n">
         <v>1.8</v>
@@ -1978,7 +1978,7 @@
         <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" t="n">
         <v>-0.5</v>
@@ -2022,7 +2022,7 @@
         <v>11</v>
       </c>
       <c r="C17" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" t="n">
         <v>0.5714285714285714</v>
@@ -2066,7 +2066,7 @@
         <v>26</v>
       </c>
       <c r="C18" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18" t="n">
         <v>1.363636363636364</v>
@@ -2110,7 +2110,7 @@
         <v>99</v>
       </c>
       <c r="C19" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D19" t="n">
         <v>2.807692307692307</v>
@@ -2154,7 +2154,7 @@
         <v>27</v>
       </c>
       <c r="C20" t="n">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D20" t="n">
         <v>-0.7272727272727273</v>
@@ -2198,7 +2198,7 @@
         <v>24</v>
       </c>
       <c r="C21" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D21" t="n">
         <v>-0.1111111111111112</v>
@@ -2242,7 +2242,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="n">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22" t="n">
         <v>-0.4583333333333334</v>
@@ -2286,7 +2286,7 @@
         <v>35</v>
       </c>
       <c r="C23" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D23" t="n">
         <v>1.692307692307693</v>
@@ -2330,7 +2330,7 @@
         <v>21</v>
       </c>
       <c r="C24" t="n">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D24" t="n">
         <v>-0.4</v>
@@ -2374,7 +2374,7 @@
         <v>77</v>
       </c>
       <c r="C25" t="n">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D25" t="n">
         <v>2.666666666666667</v>
@@ -2418,7 +2418,7 @@
         <v>150</v>
       </c>
       <c r="C26" t="n">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D26" t="n">
         <v>0.948051948051948</v>
@@ -2462,7 +2462,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D27" t="n">
         <v>-0.9333333333333333</v>
@@ -2506,7 +2506,7 @@
         <v>113</v>
       </c>
       <c r="C28" t="n">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D28" t="n">
         <v>10.3</v>
@@ -2550,7 +2550,7 @@
         <v>42</v>
       </c>
       <c r="C29" t="n">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D29" t="n">
         <v>-0.6283185840707964</v>
@@ -2594,7 +2594,7 @@
         <v>34</v>
       </c>
       <c r="C30" t="n">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D30" t="n">
         <v>-0.1904761904761905</v>
@@ -2638,7 +2638,7 @@
         <v>119</v>
       </c>
       <c r="C31" t="n">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D31" t="n">
         <v>2.5</v>
@@ -2682,7 +2682,7 @@
         <v>106</v>
       </c>
       <c r="C32" t="n">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D32" t="n">
         <v>-0.1092436974789915</v>
@@ -2726,7 +2726,7 @@
         <v>46</v>
       </c>
       <c r="C33" t="n">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D33" t="n">
         <v>-0.5660377358490566</v>
@@ -2770,7 +2770,7 @@
         <v>45</v>
       </c>
       <c r="C34" t="n">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D34" t="n">
         <v>-0.02173913043478259</v>
@@ -2814,7 +2814,7 @@
         <v>69</v>
       </c>
       <c r="C35" t="n">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D35" t="n">
         <v>0.5333333333333334</v>
@@ -2858,7 +2858,7 @@
         <v>116</v>
       </c>
       <c r="C36" t="n">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="D36" t="n">
         <v>0.681159420289855</v>
@@ -2902,7 +2902,7 @@
         <v>113</v>
       </c>
       <c r="C37" t="n">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="D37" t="n">
         <v>-0.02586206896551724</v>
@@ -2946,7 +2946,7 @@
         <v>120</v>
       </c>
       <c r="C38" t="n">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D38" t="n">
         <v>0.06194690265486735</v>
@@ -2990,7 +2990,7 @@
         <v>243</v>
       </c>
       <c r="C39" t="n">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D39" t="n">
         <v>1.025</v>
@@ -3034,7 +3034,7 @@
         <v>128</v>
       </c>
       <c r="C40" t="n">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="D40" t="n">
         <v>-0.4732510288065843</v>
@@ -3078,7 +3078,7 @@
         <v>93</v>
       </c>
       <c r="C41" t="n">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D41" t="n">
         <v>-0.2734375</v>
@@ -3122,7 +3122,7 @@
         <v>129</v>
       </c>
       <c r="C42" t="n">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="D42" t="n">
         <v>0.3870967741935485</v>
@@ -3166,7 +3166,7 @@
         <v>259</v>
       </c>
       <c r="C43" t="n">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="D43" t="n">
         <v>1.007751937984496</v>
@@ -3210,7 +3210,7 @@
         <v>218</v>
       </c>
       <c r="C44" t="n">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="D44" t="n">
         <v>-0.1583011583011583</v>
@@ -3254,7 +3254,7 @@
         <v>117</v>
       </c>
       <c r="C45" t="n">
-        <v>2687</v>
+        <v>2686</v>
       </c>
       <c r="D45" t="n">
         <v>-0.463302752293578</v>
@@ -3298,7 +3298,7 @@
         <v>189</v>
       </c>
       <c r="C46" t="n">
-        <v>2876</v>
+        <v>2875</v>
       </c>
       <c r="D46" t="n">
         <v>0.6153846153846154</v>
@@ -3342,7 +3342,7 @@
         <v>130</v>
       </c>
       <c r="C47" t="n">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="D47" t="n">
         <v>-0.3121693121693122</v>
@@ -3386,7 +3386,7 @@
         <v>250</v>
       </c>
       <c r="C48" t="n">
-        <v>3256</v>
+        <v>3255</v>
       </c>
       <c r="D48" t="n">
         <v>0.9230769230769231</v>
@@ -3430,7 +3430,7 @@
         <v>154</v>
       </c>
       <c r="C49" t="n">
-        <v>3410</v>
+        <v>3409</v>
       </c>
       <c r="D49" t="n">
         <v>-0.384</v>
@@ -3474,7 +3474,7 @@
         <v>137</v>
       </c>
       <c r="C50" t="n">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="D50" t="n">
         <v>-0.1103896103896104</v>
@@ -3515,13 +3515,13 @@
         <v>43936</v>
       </c>
       <c r="B51" t="n">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C51" t="n">
-        <v>3720</v>
+        <v>3718</v>
       </c>
       <c r="D51" t="n">
-        <v>0.2627737226277371</v>
+        <v>0.2554744525547445</v>
       </c>
       <c r="E51" t="n">
         <v>36</v>
@@ -3533,7 +3533,7 @@
         <v>2.6</v>
       </c>
       <c r="H51" t="n">
-        <v>20.8092485549133</v>
+        <v>20.93023255813954</v>
       </c>
       <c r="I51" t="n">
         <v>5</v>
@@ -3562,10 +3562,10 @@
         <v>195</v>
       </c>
       <c r="C52" t="n">
-        <v>3915</v>
+        <v>3913</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1271676300578035</v>
+        <v>0.1337209302325582</v>
       </c>
       <c r="E52" t="n">
         <v>26</v>
@@ -3606,7 +3606,7 @@
         <v>209</v>
       </c>
       <c r="C53" t="n">
-        <v>4124</v>
+        <v>4122</v>
       </c>
       <c r="D53" t="n">
         <v>0.07179487179487176</v>
@@ -3650,7 +3650,7 @@
         <v>242</v>
       </c>
       <c r="C54" t="n">
-        <v>4366</v>
+        <v>4364</v>
       </c>
       <c r="D54" t="n">
         <v>0.1578947368421053</v>
@@ -3691,13 +3691,13 @@
         <v>43940</v>
       </c>
       <c r="B55" t="n">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C55" t="n">
-        <v>4661</v>
+        <v>4658</v>
       </c>
       <c r="D55" t="n">
-        <v>0.21900826446281</v>
+        <v>0.2148760330578512</v>
       </c>
       <c r="E55" t="n">
         <v>51</v>
@@ -3709,7 +3709,7 @@
         <v>0.7</v>
       </c>
       <c r="H55" t="n">
-        <v>17.28813559322034</v>
+        <v>17.3469387755102</v>
       </c>
       <c r="I55" t="n">
         <v>9</v>
@@ -3738,10 +3738,10 @@
         <v>353</v>
       </c>
       <c r="C56" t="n">
-        <v>5014</v>
+        <v>5011</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1966101694915254</v>
+        <v>0.2006802721088434</v>
       </c>
       <c r="E56" t="n">
         <v>37</v>
@@ -3782,7 +3782,7 @@
         <v>191</v>
       </c>
       <c r="C57" t="n">
-        <v>5205</v>
+        <v>5202</v>
       </c>
       <c r="D57" t="n">
         <v>-0.4589235127478754</v>
@@ -3809,13 +3809,13 @@
         <v>-0.7619047619047619</v>
       </c>
       <c r="L57" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M57" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N57" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="58">
@@ -3826,7 +3826,7 @@
         <v>172</v>
       </c>
       <c r="C58" t="n">
-        <v>5377</v>
+        <v>5374</v>
       </c>
       <c r="D58" t="n">
         <v>-0.09947643979057597</v>
@@ -3853,13 +3853,13 @@
         <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M58" t="n">
         <v>18</v>
       </c>
       <c r="N58" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -3870,7 +3870,7 @@
         <v>255</v>
       </c>
       <c r="C59" t="n">
-        <v>5632</v>
+        <v>5629</v>
       </c>
       <c r="D59" t="n">
         <v>0.4825581395348837</v>
@@ -3903,7 +3903,7 @@
         <v>19</v>
       </c>
       <c r="N59" t="n">
-        <v>0</v>
+        <v>-0.6666666666666667</v>
       </c>
     </row>
     <row r="60">
@@ -3914,7 +3914,7 @@
         <v>263</v>
       </c>
       <c r="C60" t="n">
-        <v>5895</v>
+        <v>5892</v>
       </c>
       <c r="D60" t="n">
         <v>0.03137254901960795</v>
@@ -3955,13 +3955,13 @@
         <v>43946</v>
       </c>
       <c r="B61" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C61" t="n">
-        <v>6187</v>
+        <v>6183</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1102661596958174</v>
+        <v>0.1064638783269962</v>
       </c>
       <c r="E61" t="n">
         <v>28</v>
@@ -3973,7 +3973,7 @@
         <v>-0.1764705882352942</v>
       </c>
       <c r="H61" t="n">
-        <v>9.58904109589041</v>
+        <v>9.621993127147768</v>
       </c>
       <c r="I61" t="n">
         <v>3</v>
@@ -4002,10 +4002,10 @@
         <v>297</v>
       </c>
       <c r="C62" t="n">
-        <v>6484</v>
+        <v>6480</v>
       </c>
       <c r="D62" t="n">
-        <v>0.01712328767123283</v>
+        <v>0.02061855670103085</v>
       </c>
       <c r="E62" t="n">
         <v>32</v>
@@ -4043,13 +4043,13 @@
         <v>43948</v>
       </c>
       <c r="B63" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C63" t="n">
-        <v>6710</v>
+        <v>6705</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.2390572390572391</v>
+        <v>-0.2424242424242424</v>
       </c>
       <c r="E63" t="n">
         <v>17</v>
@@ -4061,7 +4061,7 @@
         <v>-0.46875</v>
       </c>
       <c r="H63" t="n">
-        <v>7.52212389380531</v>
+        <v>7.555555555555555</v>
       </c>
       <c r="I63" t="n">
         <v>35</v>
@@ -4090,10 +4090,10 @@
         <v>250</v>
       </c>
       <c r="C64" t="n">
-        <v>6960</v>
+        <v>6955</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1061946902654867</v>
+        <v>0.1111111111111112</v>
       </c>
       <c r="E64" t="n">
         <v>10</v>
@@ -4134,7 +4134,7 @@
         <v>225</v>
       </c>
       <c r="C65" t="n">
-        <v>7185</v>
+        <v>7180</v>
       </c>
       <c r="D65" t="n">
         <v>-0.09999999999999998</v>
@@ -4175,13 +4175,13 @@
         <v>43951</v>
       </c>
       <c r="B66" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C66" t="n">
-        <v>7428</v>
+        <v>7422</v>
       </c>
       <c r="D66" t="n">
-        <v>0.08000000000000007</v>
+        <v>0.0755555555555556</v>
       </c>
       <c r="E66" t="n">
         <v>7</v>
@@ -4193,7 +4193,7 @@
         <v>-0.2222222222222222</v>
       </c>
       <c r="H66" t="n">
-        <v>2.880658436213992</v>
+        <v>2.892561983471075</v>
       </c>
       <c r="I66" t="n">
         <v>22</v>
@@ -4222,10 +4222,10 @@
         <v>221</v>
       </c>
       <c r="C67" t="n">
-        <v>7649</v>
+        <v>7643</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.09053497942386834</v>
+        <v>-0.08677685950413228</v>
       </c>
       <c r="E67" t="n">
         <v>7</v>
@@ -4263,13 +4263,13 @@
         <v>43953</v>
       </c>
       <c r="B68" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C68" t="n">
-        <v>7880</v>
+        <v>7873</v>
       </c>
       <c r="D68" t="n">
-        <v>0.0452488687782806</v>
+        <v>0.04072398190045257</v>
       </c>
       <c r="E68" t="n">
         <v>10</v>
@@ -4281,7 +4281,7 @@
         <v>0.4285714285714286</v>
       </c>
       <c r="H68" t="n">
-        <v>4.329004329004329</v>
+        <v>4.347826086956522</v>
       </c>
       <c r="I68" t="n">
         <v>38</v>
@@ -4310,22 +4310,22 @@
         <v>412</v>
       </c>
       <c r="C69" t="n">
-        <v>8292</v>
+        <v>8285</v>
       </c>
       <c r="D69" t="n">
-        <v>0.7835497835497836</v>
+        <v>0.7913043478260871</v>
       </c>
       <c r="E69" t="n">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F69" t="n">
-        <v>834</v>
+        <v>851</v>
       </c>
       <c r="G69" t="n">
-        <v>0.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="H69" t="n">
-        <v>2.669902912621359</v>
+        <v>6.796116504854369</v>
       </c>
       <c r="I69" t="n">
         <v>45</v>
@@ -4354,7 +4354,7 @@
         <v>254</v>
       </c>
       <c r="C70" t="n">
-        <v>8546</v>
+        <v>8539</v>
       </c>
       <c r="D70" t="n">
         <v>-0.383495145631068</v>
@@ -4363,31 +4363,31 @@
         <v>4</v>
       </c>
       <c r="F70" t="n">
-        <v>838</v>
+        <v>855</v>
       </c>
       <c r="G70" t="n">
-        <v>-0.6363636363636364</v>
+        <v>-0.8571428571428572</v>
       </c>
       <c r="H70" t="n">
         <v>1.574803149606299</v>
       </c>
       <c r="I70" t="n">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="J70" t="n">
-        <v>468</v>
+        <v>403</v>
       </c>
       <c r="K70" t="n">
-        <v>0.9333333333333333</v>
+        <v>-0.5111111111111111</v>
       </c>
       <c r="L70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N70" t="n">
-        <v>-1</v>
+        <v>-0.6666666666666667</v>
       </c>
     </row>
     <row r="71">
@@ -4398,7 +4398,7 @@
         <v>220</v>
       </c>
       <c r="C71" t="n">
-        <v>8766</v>
+        <v>8759</v>
       </c>
       <c r="D71" t="n">
         <v>-0.1338582677165354</v>
@@ -4407,7 +4407,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="n">
-        <v>839</v>
+        <v>856</v>
       </c>
       <c r="G71" t="n">
         <v>-0.75</v>
@@ -4416,22 +4416,22 @@
         <v>0.4545454545454545</v>
       </c>
       <c r="I71" t="n">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="J71" t="n">
-        <v>511</v>
+        <v>490</v>
       </c>
       <c r="K71" t="n">
-        <v>-0.5057471264367817</v>
+        <v>2.954545454545455</v>
       </c>
       <c r="L71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M71" t="n">
         <v>26</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="72">
@@ -4442,7 +4442,7 @@
         <v>324</v>
       </c>
       <c r="C72" t="n">
-        <v>9090</v>
+        <v>9083</v>
       </c>
       <c r="D72" t="n">
         <v>0.4727272727272727</v>
@@ -4451,7 +4451,7 @@
         <v>4</v>
       </c>
       <c r="F72" t="n">
-        <v>843</v>
+        <v>860</v>
       </c>
       <c r="G72" t="n">
         <v>3</v>
@@ -4460,13 +4460,13 @@
         <v>1.234567901234568</v>
       </c>
       <c r="I72" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="J72" t="n">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="K72" t="n">
-        <v>-0.3488372093023255</v>
+        <v>-0.5057471264367817</v>
       </c>
       <c r="L72" t="n">
         <v>0</v>
@@ -4475,7 +4475,7 @@
         <v>26</v>
       </c>
       <c r="N72" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -4486,7 +4486,7 @@
         <v>229</v>
       </c>
       <c r="C73" t="n">
-        <v>9319</v>
+        <v>9312</v>
       </c>
       <c r="D73" t="n">
         <v>-0.2932098765432098</v>
@@ -4495,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="n">
-        <v>844</v>
+        <v>861</v>
       </c>
       <c r="G73" t="n">
         <v>-0.75</v>
@@ -4507,16 +4507,16 @@
         <v>28</v>
       </c>
       <c r="J73" t="n">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="K73" t="n">
-        <v>0</v>
+        <v>-0.3488372093023255</v>
       </c>
       <c r="L73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M73" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N73" t="n">
         <v>0</v>
@@ -4530,7 +4530,7 @@
         <v>243</v>
       </c>
       <c r="C74" t="n">
-        <v>9562</v>
+        <v>9555</v>
       </c>
       <c r="D74" t="n">
         <v>0.06113537117903922</v>
@@ -4539,7 +4539,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>845</v>
+        <v>862</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
@@ -4551,7 +4551,7 @@
         <v>61</v>
       </c>
       <c r="J74" t="n">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="K74" t="n">
         <v>1.178571428571428</v>
@@ -4560,7 +4560,7 @@
         <v>1</v>
       </c>
       <c r="M74" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N74" t="n">
         <v>0</v>
@@ -4574,7 +4574,7 @@
         <v>177</v>
       </c>
       <c r="C75" t="n">
-        <v>9739</v>
+        <v>9732</v>
       </c>
       <c r="D75" t="n">
         <v>-0.2716049382716049</v>
@@ -4583,7 +4583,7 @@
         <v>8</v>
       </c>
       <c r="F75" t="n">
-        <v>853</v>
+        <v>870</v>
       </c>
       <c r="G75" t="n">
         <v>7</v>
@@ -4595,19 +4595,19 @@
         <v>31</v>
       </c>
       <c r="J75" t="n">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="K75" t="n">
         <v>-0.4918032786885246</v>
       </c>
       <c r="L75" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M75" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N75" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="76">
@@ -4618,7 +4618,7 @@
         <v>200</v>
       </c>
       <c r="C76" t="n">
-        <v>9939</v>
+        <v>9932</v>
       </c>
       <c r="D76" t="n">
         <v>0.1299435028248588</v>
@@ -4627,7 +4627,7 @@
         <v>14</v>
       </c>
       <c r="F76" t="n">
-        <v>867</v>
+        <v>884</v>
       </c>
       <c r="G76" t="n">
         <v>0.75</v>
@@ -4639,19 +4639,19 @@
         <v>2</v>
       </c>
       <c r="J76" t="n">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="K76" t="n">
         <v>-0.935483870967742</v>
       </c>
       <c r="L76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M76" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N76" t="n">
-        <v>-0.6666666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -4659,43 +4659,43 @@
         <v>43962</v>
       </c>
       <c r="B77" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C77" t="n">
-        <v>10135</v>
+        <v>10129</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.02000000000000002</v>
+        <v>-0.01500000000000001</v>
       </c>
       <c r="E77" t="n">
         <v>11</v>
       </c>
       <c r="F77" t="n">
-        <v>878</v>
+        <v>895</v>
       </c>
       <c r="G77" t="n">
         <v>-0.2142857142857143</v>
       </c>
       <c r="H77" t="n">
-        <v>5.612244897959184</v>
+        <v>5.583756345177665</v>
       </c>
       <c r="I77" t="n">
         <v>2</v>
       </c>
       <c r="J77" t="n">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="K77" t="n">
         <v>0</v>
       </c>
       <c r="L77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M77" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -4706,16 +4706,16 @@
         <v>257</v>
       </c>
       <c r="C78" t="n">
-        <v>10392</v>
+        <v>10386</v>
       </c>
       <c r="D78" t="n">
-        <v>0.3112244897959184</v>
+        <v>0.3045685279187818</v>
       </c>
       <c r="E78" t="n">
         <v>24</v>
       </c>
       <c r="F78" t="n">
-        <v>902</v>
+        <v>919</v>
       </c>
       <c r="G78" t="n">
         <v>1.181818181818182</v>
@@ -4727,19 +4727,19 @@
         <v>14</v>
       </c>
       <c r="J78" t="n">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="K78" t="n">
         <v>6</v>
       </c>
       <c r="L78" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M78" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -4750,7 +4750,7 @@
         <v>255</v>
       </c>
       <c r="C79" t="n">
-        <v>10647</v>
+        <v>10641</v>
       </c>
       <c r="D79" t="n">
         <v>-0.007782101167315147</v>
@@ -4759,7 +4759,7 @@
         <v>8</v>
       </c>
       <c r="F79" t="n">
-        <v>910</v>
+        <v>927</v>
       </c>
       <c r="G79" t="n">
         <v>-0.6666666666666667</v>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="J79" t="n">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="K79" t="n">
         <v>-1</v>
@@ -4780,7 +4780,7 @@
         <v>0</v>
       </c>
       <c r="M79" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N79" t="n">
         <v>-1</v>
@@ -4794,7 +4794,7 @@
         <v>300</v>
       </c>
       <c r="C80" t="n">
-        <v>10947</v>
+        <v>10941</v>
       </c>
       <c r="D80" t="n">
         <v>0.1764705882352942</v>
@@ -4803,7 +4803,7 @@
         <v>18</v>
       </c>
       <c r="F80" t="n">
-        <v>928</v>
+        <v>945</v>
       </c>
       <c r="G80" t="n">
         <v>1.25</v>
@@ -4815,7 +4815,7 @@
         <v>19</v>
       </c>
       <c r="J80" t="n">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="K80" t="n">
         <v>0</v>
@@ -4824,7 +4824,7 @@
         <v>0</v>
       </c>
       <c r="M80" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N80" t="n">
         <v>0</v>
@@ -4838,7 +4838,7 @@
         <v>236</v>
       </c>
       <c r="C81" t="n">
-        <v>11183</v>
+        <v>11177</v>
       </c>
       <c r="D81" t="n">
         <v>-0.2133333333333334</v>
@@ -4847,7 +4847,7 @@
         <v>10</v>
       </c>
       <c r="F81" t="n">
-        <v>938</v>
+        <v>955</v>
       </c>
       <c r="G81" t="n">
         <v>-0.4444444444444444</v>
@@ -4859,16 +4859,16 @@
         <v>1</v>
       </c>
       <c r="J81" t="n">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="K81" t="n">
         <v>-0.9473684210526316</v>
       </c>
       <c r="L81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M81" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="N81" t="n">
         <v>0</v>
@@ -4882,7 +4882,7 @@
         <v>407</v>
       </c>
       <c r="C82" t="n">
-        <v>11590</v>
+        <v>11584</v>
       </c>
       <c r="D82" t="n">
         <v>0.7245762711864407</v>
@@ -4891,7 +4891,7 @@
         <v>23</v>
       </c>
       <c r="F82" t="n">
-        <v>961</v>
+        <v>978</v>
       </c>
       <c r="G82" t="n">
         <v>1.3</v>
@@ -4903,7 +4903,7 @@
         <v>22</v>
       </c>
       <c r="J82" t="n">
-        <v>719</v>
+        <v>713</v>
       </c>
       <c r="K82" t="n">
         <v>21</v>
@@ -4912,10 +4912,10 @@
         <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="N82" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -4926,7 +4926,7 @@
         <v>202</v>
       </c>
       <c r="C83" t="n">
-        <v>11792</v>
+        <v>11786</v>
       </c>
       <c r="D83" t="n">
         <v>-0.5036855036855037</v>
@@ -4935,7 +4935,7 @@
         <v>7</v>
       </c>
       <c r="F83" t="n">
-        <v>968</v>
+        <v>985</v>
       </c>
       <c r="G83" t="n">
         <v>-0.6956521739130435</v>
@@ -4947,16 +4947,16 @@
         <v>23</v>
       </c>
       <c r="J83" t="n">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="K83" t="n">
         <v>0.04545454545454541</v>
       </c>
       <c r="L83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M83" t="n">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N83" t="n">
         <v>0</v>
@@ -4970,7 +4970,7 @@
         <v>200</v>
       </c>
       <c r="C84" t="n">
-        <v>11992</v>
+        <v>11986</v>
       </c>
       <c r="D84" t="n">
         <v>-0.00990099009900991</v>
@@ -4979,7 +4979,7 @@
         <v>3</v>
       </c>
       <c r="F84" t="n">
-        <v>971</v>
+        <v>988</v>
       </c>
       <c r="G84" t="n">
         <v>-0.5714285714285714</v>
@@ -4991,19 +4991,19 @@
         <v>18</v>
       </c>
       <c r="J84" t="n">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="K84" t="n">
         <v>-0.2173913043478261</v>
       </c>
       <c r="L84" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M84" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="N84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -5014,7 +5014,7 @@
         <v>211</v>
       </c>
       <c r="C85" t="n">
-        <v>12203</v>
+        <v>12197</v>
       </c>
       <c r="D85" t="n">
         <v>0.05499999999999994</v>
@@ -5023,7 +5023,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>972</v>
+        <v>989</v>
       </c>
       <c r="G85" t="n">
         <v>-0.6666666666666667</v>
@@ -5035,7 +5035,7 @@
         <v>15</v>
       </c>
       <c r="J85" t="n">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="K85" t="n">
         <v>-0.1666666666666666</v>
@@ -5044,10 +5044,10 @@
         <v>0</v>
       </c>
       <c r="M85" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="N85" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Active Infections per POL request.
</commit_message>
<xml_diff>
--- a/Graphics/20200520/20200520_Kosovo_COVID.xlsx
+++ b/Graphics/20200520/20200520_Kosovo_COVID.xlsx
@@ -366,7 +366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -417,27 +417,32 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Recovered_Cum</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Recovered_Delta</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Cum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Delta</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Tested_Positive_Ratio</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Cum</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Delta</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Cum</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Delta</t>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Active_Infections</t>
         </is>
       </c>
     </row>
@@ -486,6 +491,9 @@
       <c r="N2" t="n">
         <v>14</v>
       </c>
+      <c r="O2" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -494,43 +502,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>245.5714285714286</v>
+        <v>237.2857142857143</v>
       </c>
       <c r="C3" t="n">
-        <v>9.5</v>
+        <v>10.21428571428571</v>
       </c>
       <c r="D3" t="n">
-        <v>19.92857142857143</v>
+        <v>17.07142857142857</v>
       </c>
       <c r="E3" t="n">
         <v>0.2142857142857143</v>
       </c>
       <c r="F3" t="n">
-        <v>10602.92857142857</v>
+        <v>10840.21428571429</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04356462792655074</v>
+        <v>0.008782822054697477</v>
       </c>
       <c r="H3" t="n">
-        <v>922.7142857142857</v>
+        <v>932.9285714285714</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7480481388866485</v>
+        <v>1.462333853172362</v>
       </c>
       <c r="J3" t="n">
-        <v>3.784982313396027</v>
+        <v>686.7857142857143</v>
       </c>
       <c r="K3" t="n">
-        <v>669.7142857142857</v>
+        <v>1.66546251592859</v>
       </c>
       <c r="L3" t="n">
-        <v>1.686480578325963</v>
+        <v>28.57142857142857</v>
       </c>
       <c r="M3" t="n">
-        <v>28.35714285714286</v>
+        <v>-0.1428571428571428</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.1428571428571428</v>
+        <v>4.177568122648503</v>
+      </c>
+      <c r="O3" t="n">
+        <v>246.1428571428571</v>
       </c>
     </row>
     <row r="4">
@@ -540,43 +551,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>62.06288905458879</v>
+        <v>58.42342598048067</v>
       </c>
       <c r="C4" t="n">
-        <v>7.783117824941563</v>
+        <v>7.697937500281602</v>
       </c>
       <c r="D4" t="n">
-        <v>17.28255806259054</v>
+        <v>16.46191074858886</v>
       </c>
       <c r="E4" t="n">
         <v>0.4258153136263202</v>
       </c>
       <c r="F4" t="n">
-        <v>1030.92829447622</v>
+        <v>1036.472804093949</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3197112084771773</v>
+        <v>0.2949602006991703</v>
       </c>
       <c r="H4" t="n">
-        <v>50.86698879873419</v>
+        <v>51.65635605498243</v>
       </c>
       <c r="I4" t="n">
-        <v>2.110102634057612</v>
+        <v>3.880712768796962</v>
       </c>
       <c r="J4" t="n">
-        <v>2.764455872658345</v>
+        <v>58.98654158290761</v>
       </c>
       <c r="K4" t="n">
-        <v>66.52984127607536</v>
+        <v>5.840242440035001</v>
       </c>
       <c r="L4" t="n">
-        <v>5.831209625978868</v>
+        <v>0.6462061726588642</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9287827316640653</v>
+        <v>0.3631365196012815</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3631365196012815</v>
+        <v>2.764668957459381</v>
+      </c>
+      <c r="O4" t="n">
+        <v>21.60789436527999</v>
       </c>
     </row>
     <row r="5">
@@ -598,31 +612,34 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>9083</v>
+        <v>9312</v>
       </c>
       <c r="G5" t="n">
         <v>-0.5036855036855037</v>
       </c>
       <c r="H5" t="n">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="I5" t="n">
         <v>-0.75</v>
       </c>
       <c r="J5" t="n">
+        <v>561</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>27</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N5" t="n">
         <v>0.411522633744856</v>
       </c>
-      <c r="K5" t="n">
-        <v>533</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>26</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-1</v>
+      <c r="O5" t="n">
+        <v>217</v>
       </c>
     </row>
     <row r="6">
@@ -635,40 +652,43 @@
         <v>200.5</v>
       </c>
       <c r="C6" t="n">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>2.25</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>9782</v>
+        <v>9981.25</v>
       </c>
       <c r="G6" t="n">
         <v>-0.16375</v>
       </c>
       <c r="H6" t="n">
-        <v>873.5</v>
+        <v>886.75</v>
       </c>
       <c r="I6" t="n">
         <v>-0.6428571428571428</v>
       </c>
       <c r="J6" t="n">
-        <v>1.300925925925926</v>
+        <v>655.5</v>
       </c>
       <c r="K6" t="n">
-        <v>653.5</v>
+        <v>-0.7229508196721313</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.5022611644997174</v>
+        <v>28</v>
       </c>
       <c r="M6" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1.909313725490196</v>
+      </c>
+      <c r="O6" t="n">
+        <v>231.75</v>
       </c>
     </row>
     <row r="7">
@@ -678,43 +698,46 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>232.5</v>
+        <v>220</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10513.5</v>
+        <v>10791</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0236089494163424</v>
+        <v>-0.008841545633162529</v>
       </c>
       <c r="H7" t="n">
-        <v>923</v>
+        <v>936</v>
       </c>
       <c r="I7" t="n">
         <v>-0.1071428571428572</v>
       </c>
       <c r="J7" t="n">
-        <v>3.851317335123343</v>
+        <v>680.5</v>
       </c>
       <c r="K7" t="n">
-        <v>671</v>
+        <v>-0.1920289855072463</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.1920289855072463</v>
+        <v>29</v>
       </c>
       <c r="M7" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>4.378531073446327</v>
+      </c>
+      <c r="O7" t="n">
+        <v>244</v>
       </c>
     </row>
     <row r="8">
@@ -724,43 +747,46 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>256.5</v>
+        <v>252</v>
       </c>
       <c r="C8" t="n">
-        <v>13.25</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>26.75</v>
+        <v>22.75</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>11482.25</v>
+        <v>11735.5</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1648388168826853</v>
+        <v>0.1127414699134039</v>
       </c>
       <c r="H8" t="n">
-        <v>972.25</v>
+        <v>983.25</v>
       </c>
       <c r="I8" t="n">
         <v>1.232954545454545</v>
       </c>
       <c r="J8" t="n">
-        <v>5.634268324623655</v>
+        <v>730.25</v>
       </c>
       <c r="K8" t="n">
-        <v>707.5</v>
+        <v>0.03409090909090906</v>
       </c>
       <c r="L8" t="n">
-        <v>0.03409090909090906</v>
+        <v>29</v>
       </c>
       <c r="M8" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>5.912776412776413</v>
+      </c>
+      <c r="O8" t="n">
+        <v>255.75</v>
       </c>
     </row>
     <row r="9">
@@ -782,31 +808,34 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>12197</v>
+        <v>12405</v>
       </c>
       <c r="G9" t="n">
         <v>0.7245762711864407</v>
       </c>
       <c r="H9" t="n">
-        <v>989</v>
+        <v>1003</v>
       </c>
       <c r="I9" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J9" t="n">
+        <v>772</v>
+      </c>
+      <c r="K9" t="n">
+        <v>21</v>
+      </c>
+      <c r="L9" t="n">
+        <v>29</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
         <v>9.338521400778211</v>
       </c>
-      <c r="K9" t="n">
-        <v>769</v>
-      </c>
-      <c r="L9" t="n">
-        <v>21</v>
-      </c>
-      <c r="M9" t="n">
-        <v>29</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
+      <c r="O9" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -820,7 +849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,27 +900,32 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Recovered_Cum</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Recovered_Delta</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Cum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Delta</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Tested_Positive_Ratio</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Cum</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Delta</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Cum</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Delta</t>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Active_Infections</t>
         </is>
       </c>
     </row>
@@ -902,43 +936,46 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M2" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N2" t="n">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="O2" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="3">
@@ -948,43 +985,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>145.202380952381</v>
+        <v>145.9411764705882</v>
       </c>
       <c r="C3" t="n">
-        <v>11.77380952380952</v>
+        <v>11.8</v>
       </c>
       <c r="D3" t="n">
-        <v>9.154761904761905</v>
+        <v>9.08235294117647</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3452380952380952</v>
+        <v>0.3411764705882353</v>
       </c>
       <c r="F3" t="n">
-        <v>3871.595238095238</v>
+        <v>3971.988235294118</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3662432723157148</v>
+        <v>0.3617672572357808</v>
       </c>
       <c r="H3" t="n">
-        <v>374.9761904761905</v>
+        <v>382.364705882353</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6605708486938211</v>
+        <v>0.8057406034150701</v>
       </c>
       <c r="J3" t="n">
-        <v>7.317510264686279</v>
+        <v>176.4588235294118</v>
       </c>
       <c r="K3" t="n">
-        <v>169.3690476190476</v>
+        <v>0.920729251955945</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9412141240030396</v>
+        <v>10.48235294117647</v>
       </c>
       <c r="M3" t="n">
-        <v>10.26190476190476</v>
+        <v>-0.1333333333333333</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.1349206349206349</v>
+        <v>7.310607428993138</v>
+      </c>
+      <c r="O3" t="n">
+        <v>205.9058823529412</v>
       </c>
     </row>
     <row r="4">
@@ -994,43 +1034,46 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>109.9938420797618</v>
+        <v>109.549114114909</v>
       </c>
       <c r="C4" t="n">
-        <v>14.38234459033328</v>
+        <v>14.29851807173103</v>
       </c>
       <c r="D4" t="n">
-        <v>15.28326437061617</v>
+        <v>15.20668067840256</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7196727438845412</v>
+        <v>0.7163555444794457</v>
       </c>
       <c r="F4" t="n">
-        <v>3930.157316570051</v>
+        <v>4014.840972638173</v>
       </c>
       <c r="G4" t="n">
-        <v>1.350534704742466</v>
+        <v>1.34310584848522</v>
       </c>
       <c r="H4" t="n">
-        <v>371.3236816238768</v>
+        <v>375.3398411553767</v>
       </c>
       <c r="I4" t="n">
-        <v>2.135947705410573</v>
+        <v>2.509835001447996</v>
       </c>
       <c r="J4" t="n">
-        <v>7.65604245748536</v>
+        <v>255.4890060509163</v>
       </c>
       <c r="K4" t="n">
-        <v>248.469473035235</v>
+        <v>4.617812147439339</v>
       </c>
       <c r="L4" t="n">
-        <v>4.641660121019395</v>
+        <v>11.45967231799645</v>
       </c>
       <c r="M4" t="n">
-        <v>11.34573753369923</v>
+        <v>0.3598574085625504</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3617192607698794</v>
+        <v>7.610600425332406</v>
+      </c>
+      <c r="O4" t="n">
+        <v>189.5521428154754</v>
       </c>
     </row>
     <row r="5">
@@ -1067,16 +1110,19 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
         <v>-1</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" t="n">
-        <v>-1</v>
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1086,7 +1132,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>26.75</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -1098,31 +1144,34 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>309.25</v>
+        <v>318</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.2206060606060606</v>
+        <v>-0.2133333333333334</v>
       </c>
       <c r="H6" t="n">
-        <v>19.75</v>
+        <v>20</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.3529411764705882</v>
+        <v>-0.3333333333333334</v>
       </c>
       <c r="J6" t="n">
-        <v>1.134259259259259</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.175</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1.234567901234568</v>
+      </c>
+      <c r="O6" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -1132,43 +1181,46 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>143.5</v>
+        <v>150</v>
       </c>
       <c r="C7" t="n">
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>2460</v>
+        <v>2569</v>
       </c>
       <c r="G7" t="n">
-        <v>0.06154113691695329</v>
+        <v>0.06113537117903922</v>
       </c>
       <c r="H7" t="n">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>4.714285714285714</v>
+        <v>37</v>
       </c>
       <c r="K7" t="n">
-        <v>33.5</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M7" t="n">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>4.761904761904762</v>
+      </c>
+      <c r="O7" t="n">
+        <v>187</v>
       </c>
     </row>
     <row r="8">
@@ -1178,10 +1230,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>231.5</v>
+        <v>230</v>
       </c>
       <c r="C8" t="n">
-        <v>18.25</v>
+        <v>18</v>
       </c>
       <c r="D8" t="n">
         <v>14</v>
@@ -1190,31 +1242,34 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>7011.25</v>
+        <v>7180</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5428571428571429</v>
+        <v>0.5333333333333334</v>
       </c>
       <c r="H8" t="n">
-        <v>792.25</v>
+        <v>799</v>
       </c>
       <c r="I8" t="n">
-        <v>0.78125</v>
+        <v>0.875</v>
       </c>
       <c r="J8" t="n">
-        <v>11.67064662639884</v>
+        <v>249</v>
       </c>
       <c r="K8" t="n">
-        <v>236.25</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01136363636363635</v>
+        <v>22</v>
       </c>
       <c r="M8" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>11.50442477876106</v>
+      </c>
+      <c r="O8" t="n">
+        <v>327</v>
       </c>
     </row>
     <row r="9">
@@ -1236,31 +1291,34 @@
         <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>12197</v>
+        <v>12405</v>
       </c>
       <c r="G9" t="n">
         <v>10.3</v>
       </c>
       <c r="H9" t="n">
-        <v>989</v>
+        <v>1003</v>
       </c>
       <c r="I9" t="n">
         <v>13</v>
       </c>
       <c r="J9" t="n">
+        <v>772</v>
+      </c>
+      <c r="K9" t="n">
+        <v>34</v>
+      </c>
+      <c r="L9" t="n">
+        <v>29</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="n">
         <v>31.6</v>
       </c>
-      <c r="K9" t="n">
-        <v>769</v>
-      </c>
-      <c r="L9" t="n">
-        <v>34</v>
-      </c>
-      <c r="M9" t="n">
-        <v>29</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1</v>
+      <c r="O9" t="n">
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -1274,7 +1332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,37 +1378,42 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Recovered_Raw</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Recovered_Cum</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Recovered_Delta</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Raw</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Cum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Died_Delta</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Tested_Positive_Ratio</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Raw</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Cum</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Recovered_Delta</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Raw</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Cum</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Died_Delta</t>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Active_Infections</t>
         </is>
       </c>
     </row>
@@ -1397,6 +1460,9 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1441,6 +1507,9 @@
       <c r="N3" t="n">
         <v>0</v>
       </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -1485,6 +1554,9 @@
       <c r="N4" t="n">
         <v>0</v>
       </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -1529,6 +1601,9 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -1573,6 +1648,9 @@
       <c r="N6" t="n">
         <v>0</v>
       </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -1617,6 +1695,9 @@
       <c r="N7" t="n">
         <v>0</v>
       </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1661,6 +1742,9 @@
       <c r="N8" t="n">
         <v>0</v>
       </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1705,6 +1789,9 @@
       <c r="N9" t="n">
         <v>0</v>
       </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1749,6 +1836,9 @@
       <c r="N10" t="n">
         <v>0</v>
       </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1793,6 +1883,9 @@
       <c r="N11" t="n">
         <v>0</v>
       </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1837,6 +1930,9 @@
       <c r="N12" t="n">
         <v>0</v>
       </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1881,6 +1977,9 @@
       <c r="N13" t="n">
         <v>0</v>
       </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1925,6 +2024,9 @@
       <c r="N14" t="n">
         <v>0</v>
       </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1969,6 +2071,9 @@
       <c r="N15" t="n">
         <v>0</v>
       </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -2013,6 +2118,9 @@
       <c r="N16" t="n">
         <v>0</v>
       </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -2057,6 +2165,9 @@
       <c r="N17" t="n">
         <v>0</v>
       </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -2081,25 +2192,28 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
         <v>7.692307692307693</v>
       </c>
-      <c r="I18" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0</v>
+      <c r="O18" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -2125,25 +2239,28 @@
         <v>0.5</v>
       </c>
       <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" t="n">
         <v>3.03030303030303</v>
       </c>
-      <c r="I19" t="n">
-        <v>0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0</v>
+      <c r="O19" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -2169,25 +2286,28 @@
         <v>1.666666666666667</v>
       </c>
       <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" t="n">
         <v>29.62962962962963</v>
       </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0</v>
+      <c r="O20" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -2213,25 +2333,28 @@
         <v>-0.625</v>
       </c>
       <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
         <v>12.5</v>
       </c>
-      <c r="I21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0</v>
+      <c r="O21" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -2257,25 +2380,28 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" t="n">
         <v>23.07692307692308</v>
       </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0</v>
+      <c r="O22" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="23">
@@ -2301,25 +2427,28 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" t="n">
         <v>2.857142857142857</v>
       </c>
-      <c r="I23" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
+      <c r="O23" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="24">
@@ -2345,25 +2474,28 @@
         <v>0</v>
       </c>
       <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
         <v>4.761904761904762</v>
       </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0</v>
+      <c r="O24" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="25">
@@ -2389,25 +2521,28 @@
         <v>2</v>
       </c>
       <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" t="n">
         <v>3.896103896103896</v>
       </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
+      <c r="O25" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -2433,25 +2568,28 @@
         <v>1.333333333333333</v>
       </c>
       <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
         <v>4.666666666666667</v>
       </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
+      <c r="O26" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="27">
@@ -2477,25 +2615,28 @@
         <v>-0.7142857142857143</v>
       </c>
       <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
         <v>20</v>
       </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" t="n">
-        <v>1</v>
-      </c>
-      <c r="M27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N27" t="n">
-        <v>0</v>
+      <c r="O27" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="28">
@@ -2521,25 +2662,28 @@
         <v>13</v>
       </c>
       <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N28" t="n">
         <v>24.7787610619469</v>
       </c>
-      <c r="I28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>1</v>
-      </c>
-      <c r="N28" t="n">
-        <v>-1</v>
+      <c r="O28" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="29">
@@ -2565,25 +2709,28 @@
         <v>-0.9285714285714286</v>
       </c>
       <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" t="n">
         <v>4.761904761904762</v>
       </c>
-      <c r="I29" t="n">
-        <v>0</v>
-      </c>
-      <c r="J29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" t="n">
-        <v>1</v>
-      </c>
-      <c r="N29" t="n">
-        <v>0</v>
+      <c r="O29" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="30">
@@ -2609,25 +2756,28 @@
         <v>3</v>
       </c>
       <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
         <v>23.52941176470588</v>
       </c>
-      <c r="I30" t="n">
-        <v>0</v>
-      </c>
-      <c r="J30" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" t="n">
-        <v>1</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
+      <c r="O30" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="31">
@@ -2653,25 +2803,28 @@
         <v>0.875</v>
       </c>
       <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
         <v>12.60504201680672</v>
       </c>
-      <c r="I31" t="n">
-        <v>1</v>
-      </c>
-      <c r="J31" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>1</v>
-      </c>
-      <c r="N31" t="n">
-        <v>0</v>
+      <c r="O31" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="32">
@@ -2697,25 +2850,28 @@
         <v>-0.8666666666666667</v>
       </c>
       <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
         <v>1.886792452830189</v>
       </c>
-      <c r="I32" t="n">
-        <v>0</v>
-      </c>
-      <c r="J32" t="n">
-        <v>1</v>
-      </c>
-      <c r="K32" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
-        <v>1</v>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
+      <c r="O32" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="33">
@@ -2741,25 +2897,28 @@
         <v>0.5</v>
       </c>
       <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
         <v>6.521739130434782</v>
       </c>
-      <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>1</v>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
+      <c r="O33" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="34">
@@ -2785,25 +2944,28 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
         <v>6.666666666666667</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J34" t="n">
-        <v>1</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" t="n">
-        <v>1</v>
-      </c>
-      <c r="N34" t="n">
-        <v>0</v>
+      <c r="O34" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="35">
@@ -2829,25 +2991,28 @@
         <v>3</v>
       </c>
       <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
         <v>17.39130434782609</v>
       </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>1</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>1</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
+      <c r="O35" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="36">
@@ -2873,25 +3038,28 @@
         <v>-0.5</v>
       </c>
       <c r="H36" t="n">
+        <v>5</v>
+      </c>
+      <c r="I36" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
         <v>5.172413793103448</v>
       </c>
-      <c r="I36" t="n">
-        <v>5</v>
-      </c>
-      <c r="J36" t="n">
-        <v>6</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" t="n">
-        <v>1</v>
-      </c>
-      <c r="N36" t="n">
-        <v>0</v>
+      <c r="O36" t="n">
+        <v>106</v>
       </c>
     </row>
     <row r="37">
@@ -2917,25 +3085,28 @@
         <v>1.166666666666667</v>
       </c>
       <c r="H37" t="n">
+        <v>4</v>
+      </c>
+      <c r="I37" t="n">
+        <v>10</v>
+      </c>
+      <c r="J37" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>1</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
         <v>11.50442477876106</v>
       </c>
-      <c r="I37" t="n">
-        <v>4</v>
-      </c>
-      <c r="J37" t="n">
-        <v>10</v>
-      </c>
-      <c r="K37" t="n">
-        <v>-0.2</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>1</v>
-      </c>
-      <c r="N37" t="n">
-        <v>0</v>
+      <c r="O37" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="38">
@@ -2961,25 +3132,28 @@
         <v>-0.9230769230769231</v>
       </c>
       <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>10</v>
+      </c>
+      <c r="J38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
         <v>0.8333333333333334</v>
       </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="n">
-        <v>10</v>
-      </c>
-      <c r="K38" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" t="n">
-        <v>1</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0</v>
+      <c r="O38" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="39">
@@ -3005,25 +3179,28 @@
         <v>8</v>
       </c>
       <c r="H39" t="n">
+        <v>6</v>
+      </c>
+      <c r="I39" t="n">
+        <v>16</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
         <v>3.703703703703703</v>
       </c>
-      <c r="I39" t="n">
-        <v>6</v>
-      </c>
-      <c r="J39" t="n">
-        <v>16</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>1</v>
-      </c>
-      <c r="N39" t="n">
-        <v>0</v>
+      <c r="O39" t="n">
+        <v>119</v>
       </c>
     </row>
     <row r="40">
@@ -3049,25 +3226,28 @@
         <v>-0.4444444444444444</v>
       </c>
       <c r="H40" t="n">
+        <v>7</v>
+      </c>
+      <c r="I40" t="n">
+        <v>23</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>1</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" t="n">
         <v>3.90625</v>
       </c>
-      <c r="I40" t="n">
-        <v>7</v>
-      </c>
-      <c r="J40" t="n">
-        <v>23</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
-        <v>1</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0</v>
+      <c r="O40" t="n">
+        <v>117</v>
       </c>
     </row>
     <row r="41">
@@ -3093,25 +3273,28 @@
         <v>0</v>
       </c>
       <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>23</v>
+      </c>
+      <c r="J41" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>1</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" t="n">
         <v>5.376344086021505</v>
       </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>23</v>
-      </c>
-      <c r="K41" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>1</v>
-      </c>
-      <c r="N41" t="n">
-        <v>0</v>
+      <c r="O41" t="n">
+        <v>122</v>
       </c>
     </row>
     <row r="42">
@@ -3137,25 +3320,28 @@
         <v>3</v>
       </c>
       <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>24</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>2</v>
+      </c>
+      <c r="L42" t="n">
+        <v>3</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
         <v>15.50387596899225</v>
       </c>
-      <c r="I42" t="n">
-        <v>1</v>
-      </c>
-      <c r="J42" t="n">
-        <v>24</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="n">
-        <v>2</v>
-      </c>
-      <c r="M42" t="n">
-        <v>3</v>
-      </c>
-      <c r="N42" t="n">
-        <v>0</v>
+      <c r="O42" t="n">
+        <v>141</v>
       </c>
     </row>
     <row r="43">
@@ -3181,25 +3367,28 @@
         <v>-0.05000000000000004</v>
       </c>
       <c r="H43" t="n">
+        <v>6</v>
+      </c>
+      <c r="I43" t="n">
+        <v>30</v>
+      </c>
+      <c r="J43" t="n">
+        <v>5</v>
+      </c>
+      <c r="K43" t="n">
+        <v>2</v>
+      </c>
+      <c r="L43" t="n">
+        <v>5</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
         <v>7.335907335907336</v>
       </c>
-      <c r="I43" t="n">
-        <v>6</v>
-      </c>
-      <c r="J43" t="n">
-        <v>30</v>
-      </c>
-      <c r="K43" t="n">
-        <v>5</v>
-      </c>
-      <c r="L43" t="n">
-        <v>2</v>
-      </c>
-      <c r="M43" t="n">
-        <v>5</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
+      <c r="O43" t="n">
+        <v>154</v>
       </c>
     </row>
     <row r="44">
@@ -3225,25 +3414,28 @@
         <v>1.105263157894737</v>
       </c>
       <c r="H44" t="n">
+        <v>7</v>
+      </c>
+      <c r="I44" t="n">
+        <v>37</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" t="n">
+        <v>6</v>
+      </c>
+      <c r="M44" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="N44" t="n">
         <v>18.34862385321101</v>
       </c>
-      <c r="I44" t="n">
-        <v>7</v>
-      </c>
-      <c r="J44" t="n">
-        <v>37</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="L44" t="n">
-        <v>1</v>
-      </c>
-      <c r="M44" t="n">
-        <v>6</v>
-      </c>
-      <c r="N44" t="n">
-        <v>-0.5</v>
+      <c r="O44" t="n">
+        <v>187</v>
       </c>
     </row>
     <row r="45">
@@ -3269,25 +3461,28 @@
         <v>-0.925</v>
       </c>
       <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>38</v>
+      </c>
+      <c r="J45" t="n">
+        <v>-0.8571428571428572</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" t="n">
+        <v>7</v>
+      </c>
+      <c r="M45" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" t="n">
         <v>2.564102564102564</v>
       </c>
-      <c r="I45" t="n">
-        <v>1</v>
-      </c>
-      <c r="J45" t="n">
-        <v>38</v>
-      </c>
-      <c r="K45" t="n">
-        <v>-0.8571428571428572</v>
-      </c>
-      <c r="L45" t="n">
-        <v>1</v>
-      </c>
-      <c r="M45" t="n">
-        <v>7</v>
-      </c>
-      <c r="N45" t="n">
-        <v>0</v>
+      <c r="O45" t="n">
+        <v>189</v>
       </c>
     </row>
     <row r="46">
@@ -3313,25 +3508,28 @@
         <v>6.666666666666667</v>
       </c>
       <c r="H46" t="n">
+        <v>14</v>
+      </c>
+      <c r="I46" t="n">
+        <v>52</v>
+      </c>
+      <c r="J46" t="n">
+        <v>13</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>7</v>
+      </c>
+      <c r="M46" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N46" t="n">
         <v>12.16931216931217</v>
       </c>
-      <c r="I46" t="n">
-        <v>14</v>
-      </c>
-      <c r="J46" t="n">
-        <v>52</v>
-      </c>
-      <c r="K46" t="n">
-        <v>13</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>7</v>
-      </c>
-      <c r="N46" t="n">
-        <v>-1</v>
+      <c r="O46" t="n">
+        <v>198</v>
       </c>
     </row>
     <row r="47">
@@ -3357,25 +3555,28 @@
         <v>0.4347826086956521</v>
       </c>
       <c r="H47" t="n">
+        <v>6</v>
+      </c>
+      <c r="I47" t="n">
+        <v>58</v>
+      </c>
+      <c r="J47" t="n">
+        <v>-0.5714285714285714</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>7</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0</v>
+      </c>
+      <c r="N47" t="n">
         <v>25.38461538461538</v>
       </c>
-      <c r="I47" t="n">
-        <v>6</v>
-      </c>
-      <c r="J47" t="n">
-        <v>58</v>
-      </c>
-      <c r="K47" t="n">
-        <v>-0.5714285714285714</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" t="n">
-        <v>7</v>
-      </c>
-      <c r="N47" t="n">
-        <v>0</v>
+      <c r="O47" t="n">
+        <v>225</v>
       </c>
     </row>
     <row r="48">
@@ -3401,25 +3602,28 @@
         <v>1.393939393939394</v>
       </c>
       <c r="H48" t="n">
+        <v>1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>59</v>
+      </c>
+      <c r="J48" t="n">
+        <v>-0.8333333333333334</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>7</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" t="n">
         <v>31.6</v>
       </c>
-      <c r="I48" t="n">
-        <v>1</v>
-      </c>
-      <c r="J48" t="n">
-        <v>59</v>
-      </c>
-      <c r="K48" t="n">
-        <v>-0.8333333333333334</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" t="n">
-        <v>7</v>
-      </c>
-      <c r="N48" t="n">
-        <v>0</v>
+      <c r="O48" t="n">
+        <v>303</v>
       </c>
     </row>
     <row r="49">
@@ -3445,25 +3649,28 @@
         <v>-0.810126582278481</v>
       </c>
       <c r="H49" t="n">
+        <v>4</v>
+      </c>
+      <c r="I49" t="n">
+        <v>63</v>
+      </c>
+      <c r="J49" t="n">
+        <v>3</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1</v>
+      </c>
+      <c r="L49" t="n">
+        <v>8</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" t="n">
         <v>9.740259740259742</v>
       </c>
-      <c r="I49" t="n">
-        <v>4</v>
-      </c>
-      <c r="J49" t="n">
-        <v>63</v>
-      </c>
-      <c r="K49" t="n">
-        <v>3</v>
-      </c>
-      <c r="L49" t="n">
-        <v>1</v>
-      </c>
-      <c r="M49" t="n">
-        <v>8</v>
-      </c>
-      <c r="N49" t="n">
-        <v>0</v>
+      <c r="O49" t="n">
+        <v>314</v>
       </c>
     </row>
     <row r="50">
@@ -3489,25 +3696,28 @@
         <v>-0.3333333333333334</v>
       </c>
       <c r="H50" t="n">
+        <v>3</v>
+      </c>
+      <c r="I50" t="n">
+        <v>66</v>
+      </c>
+      <c r="J50" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>8</v>
+      </c>
+      <c r="M50" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N50" t="n">
         <v>7.2992700729927</v>
       </c>
-      <c r="I50" t="n">
-        <v>3</v>
-      </c>
-      <c r="J50" t="n">
-        <v>66</v>
-      </c>
-      <c r="K50" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0</v>
-      </c>
-      <c r="M50" t="n">
-        <v>8</v>
-      </c>
-      <c r="N50" t="n">
-        <v>-1</v>
+      <c r="O50" t="n">
+        <v>321</v>
       </c>
     </row>
     <row r="51">
@@ -3533,25 +3743,28 @@
         <v>2.6</v>
       </c>
       <c r="H51" t="n">
+        <v>5</v>
+      </c>
+      <c r="I51" t="n">
+        <v>71</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1</v>
+      </c>
+      <c r="L51" t="n">
+        <v>9</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" t="n">
         <v>20.93023255813954</v>
       </c>
-      <c r="I51" t="n">
-        <v>5</v>
-      </c>
-      <c r="J51" t="n">
-        <v>71</v>
-      </c>
-      <c r="K51" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="L51" t="n">
-        <v>1</v>
-      </c>
-      <c r="M51" t="n">
-        <v>9</v>
-      </c>
-      <c r="N51" t="n">
-        <v>0</v>
+      <c r="O51" t="n">
+        <v>352</v>
       </c>
     </row>
     <row r="52">
@@ -3577,25 +3790,28 @@
         <v>-0.2777777777777778</v>
       </c>
       <c r="H52" t="n">
+        <v>8</v>
+      </c>
+      <c r="I52" t="n">
+        <v>79</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="K52" t="n">
+        <v>2</v>
+      </c>
+      <c r="L52" t="n">
+        <v>11</v>
+      </c>
+      <c r="M52" t="n">
+        <v>1</v>
+      </c>
+      <c r="N52" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="I52" t="n">
-        <v>8</v>
-      </c>
-      <c r="J52" t="n">
-        <v>79</v>
-      </c>
-      <c r="K52" t="n">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="L52" t="n">
-        <v>2</v>
-      </c>
-      <c r="M52" t="n">
-        <v>11</v>
-      </c>
-      <c r="N52" t="n">
-        <v>1</v>
+      <c r="O52" t="n">
+        <v>370</v>
       </c>
     </row>
     <row r="53">
@@ -3621,25 +3837,28 @@
         <v>0.1923076923076923</v>
       </c>
       <c r="H53" t="n">
+        <v>5</v>
+      </c>
+      <c r="I53" t="n">
+        <v>84</v>
+      </c>
+      <c r="J53" t="n">
+        <v>-0.375</v>
+      </c>
+      <c r="K53" t="n">
+        <v>1</v>
+      </c>
+      <c r="L53" t="n">
+        <v>12</v>
+      </c>
+      <c r="M53" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="N53" t="n">
         <v>14.83253588516746</v>
       </c>
-      <c r="I53" t="n">
-        <v>5</v>
-      </c>
-      <c r="J53" t="n">
-        <v>84</v>
-      </c>
-      <c r="K53" t="n">
-        <v>-0.375</v>
-      </c>
-      <c r="L53" t="n">
-        <v>1</v>
-      </c>
-      <c r="M53" t="n">
-        <v>12</v>
-      </c>
-      <c r="N53" t="n">
-        <v>-0.5</v>
+      <c r="O53" t="n">
+        <v>396</v>
       </c>
     </row>
     <row r="54">
@@ -3665,25 +3884,28 @@
         <v>-0.032258064516129</v>
       </c>
       <c r="H54" t="n">
+        <v>9</v>
+      </c>
+      <c r="I54" t="n">
+        <v>93</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>12</v>
+      </c>
+      <c r="M54" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N54" t="n">
         <v>12.39669421487603</v>
       </c>
-      <c r="I54" t="n">
-        <v>9</v>
-      </c>
-      <c r="J54" t="n">
-        <v>93</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>12</v>
-      </c>
-      <c r="N54" t="n">
-        <v>-1</v>
+      <c r="O54" t="n">
+        <v>417</v>
       </c>
     </row>
     <row r="55">
@@ -3709,25 +3931,28 @@
         <v>0.7</v>
       </c>
       <c r="H55" t="n">
+        <v>9</v>
+      </c>
+      <c r="I55" t="n">
+        <v>102</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>12</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" t="n">
         <v>17.3469387755102</v>
       </c>
-      <c r="I55" t="n">
-        <v>9</v>
-      </c>
-      <c r="J55" t="n">
-        <v>102</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" t="n">
-        <v>12</v>
-      </c>
-      <c r="N55" t="n">
-        <v>0</v>
+      <c r="O55" t="n">
+        <v>459</v>
       </c>
     </row>
     <row r="56">
@@ -3753,25 +3978,28 @@
         <v>-0.2745098039215687</v>
       </c>
       <c r="H56" t="n">
+        <v>21</v>
+      </c>
+      <c r="I56" t="n">
+        <v>123</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="K56" t="n">
+        <v>3</v>
+      </c>
+      <c r="L56" t="n">
+        <v>15</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="n">
         <v>10.48158640226629</v>
       </c>
-      <c r="I56" t="n">
-        <v>21</v>
-      </c>
-      <c r="J56" t="n">
-        <v>123</v>
-      </c>
-      <c r="K56" t="n">
-        <v>1.333333333333333</v>
-      </c>
-      <c r="L56" t="n">
-        <v>3</v>
-      </c>
-      <c r="M56" t="n">
-        <v>15</v>
-      </c>
-      <c r="N56" t="n">
-        <v>0</v>
+      <c r="O56" t="n">
+        <v>475</v>
       </c>
     </row>
     <row r="57">
@@ -3797,25 +4025,28 @@
         <v>-0.8378378378378378</v>
       </c>
       <c r="H57" t="n">
+        <v>5</v>
+      </c>
+      <c r="I57" t="n">
+        <v>128</v>
+      </c>
+      <c r="J57" t="n">
+        <v>-0.7619047619047619</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>15</v>
+      </c>
+      <c r="M57" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N57" t="n">
         <v>3.141361256544502</v>
       </c>
-      <c r="I57" t="n">
-        <v>5</v>
-      </c>
-      <c r="J57" t="n">
-        <v>128</v>
-      </c>
-      <c r="K57" t="n">
-        <v>-0.7619047619047619</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0</v>
-      </c>
-      <c r="M57" t="n">
-        <v>15</v>
-      </c>
-      <c r="N57" t="n">
-        <v>-1</v>
+      <c r="O57" t="n">
+        <v>476</v>
       </c>
     </row>
     <row r="58">
@@ -3841,25 +4072,28 @@
         <v>3.333333333333333</v>
       </c>
       <c r="H58" t="n">
+        <v>10</v>
+      </c>
+      <c r="I58" t="n">
+        <v>138</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="n">
+        <v>3</v>
+      </c>
+      <c r="L58" t="n">
+        <v>18</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" t="n">
         <v>15.11627906976744</v>
       </c>
-      <c r="I58" t="n">
-        <v>10</v>
-      </c>
-      <c r="J58" t="n">
-        <v>138</v>
-      </c>
-      <c r="K58" t="n">
-        <v>1</v>
-      </c>
-      <c r="L58" t="n">
-        <v>3</v>
-      </c>
-      <c r="M58" t="n">
-        <v>18</v>
-      </c>
-      <c r="N58" t="n">
-        <v>0</v>
+      <c r="O58" t="n">
+        <v>492</v>
       </c>
     </row>
     <row r="59">
@@ -3885,25 +4119,28 @@
         <v>0.5</v>
       </c>
       <c r="H59" t="n">
+        <v>21</v>
+      </c>
+      <c r="I59" t="n">
+        <v>159</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K59" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" t="n">
+        <v>19</v>
+      </c>
+      <c r="M59" t="n">
+        <v>-0.6666666666666667</v>
+      </c>
+      <c r="N59" t="n">
         <v>15.29411764705882</v>
       </c>
-      <c r="I59" t="n">
-        <v>21</v>
-      </c>
-      <c r="J59" t="n">
-        <v>159</v>
-      </c>
-      <c r="K59" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="L59" t="n">
-        <v>1</v>
-      </c>
-      <c r="M59" t="n">
-        <v>19</v>
-      </c>
-      <c r="N59" t="n">
-        <v>-0.6666666666666667</v>
+      <c r="O59" t="n">
+        <v>510</v>
       </c>
     </row>
     <row r="60">
@@ -3929,25 +4166,28 @@
         <v>-0.1282051282051282</v>
       </c>
       <c r="H60" t="n">
+        <v>3</v>
+      </c>
+      <c r="I60" t="n">
+        <v>162</v>
+      </c>
+      <c r="J60" t="n">
+        <v>-0.8571428571428572</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>19</v>
+      </c>
+      <c r="M60" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N60" t="n">
         <v>12.92775665399239</v>
       </c>
-      <c r="I60" t="n">
-        <v>3</v>
-      </c>
-      <c r="J60" t="n">
-        <v>162</v>
-      </c>
-      <c r="K60" t="n">
-        <v>-0.8571428571428572</v>
-      </c>
-      <c r="L60" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" t="n">
-        <v>19</v>
-      </c>
-      <c r="N60" t="n">
-        <v>-1</v>
+      <c r="O60" t="n">
+        <v>541</v>
       </c>
     </row>
     <row r="61">
@@ -3973,25 +4213,28 @@
         <v>-0.1764705882352942</v>
       </c>
       <c r="H61" t="n">
+        <v>3</v>
+      </c>
+      <c r="I61" t="n">
+        <v>165</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>1</v>
+      </c>
+      <c r="L61" t="n">
+        <v>20</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" t="n">
         <v>9.621993127147768</v>
       </c>
-      <c r="I61" t="n">
-        <v>3</v>
-      </c>
-      <c r="J61" t="n">
-        <v>165</v>
-      </c>
-      <c r="K61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" t="n">
-        <v>1</v>
-      </c>
-      <c r="M61" t="n">
-        <v>20</v>
-      </c>
-      <c r="N61" t="n">
-        <v>0</v>
+      <c r="O61" t="n">
+        <v>566</v>
       </c>
     </row>
     <row r="62">
@@ -4017,25 +4260,28 @@
         <v>0.1428571428571428</v>
       </c>
       <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
+        <v>166</v>
+      </c>
+      <c r="J62" t="n">
+        <v>-0.6666666666666667</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" t="n">
+        <v>21</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" t="n">
         <v>10.77441077441077</v>
       </c>
-      <c r="I62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" t="n">
-        <v>166</v>
-      </c>
-      <c r="K62" t="n">
-        <v>-0.6666666666666667</v>
-      </c>
-      <c r="L62" t="n">
-        <v>1</v>
-      </c>
-      <c r="M62" t="n">
-        <v>21</v>
-      </c>
-      <c r="N62" t="n">
-        <v>0</v>
+      <c r="O62" t="n">
+        <v>597</v>
       </c>
     </row>
     <row r="63">
@@ -4061,25 +4307,28 @@
         <v>-0.46875</v>
       </c>
       <c r="H63" t="n">
+        <v>35</v>
+      </c>
+      <c r="I63" t="n">
+        <v>201</v>
+      </c>
+      <c r="J63" t="n">
+        <v>34</v>
+      </c>
+      <c r="K63" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
+        <v>22</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" t="n">
         <v>7.555555555555555</v>
       </c>
-      <c r="I63" t="n">
-        <v>35</v>
-      </c>
-      <c r="J63" t="n">
-        <v>201</v>
-      </c>
-      <c r="K63" t="n">
-        <v>34</v>
-      </c>
-      <c r="L63" t="n">
-        <v>1</v>
-      </c>
-      <c r="M63" t="n">
-        <v>22</v>
-      </c>
-      <c r="N63" t="n">
-        <v>0</v>
+      <c r="O63" t="n">
+        <v>579</v>
       </c>
     </row>
     <row r="64">
@@ -4105,25 +4354,28 @@
         <v>-0.4117647058823529</v>
       </c>
       <c r="H64" t="n">
+        <v>31</v>
+      </c>
+      <c r="I64" t="n">
+        <v>232</v>
+      </c>
+      <c r="J64" t="n">
+        <v>-0.1142857142857143</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" t="n">
+        <v>22</v>
+      </c>
+      <c r="M64" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N64" t="n">
         <v>4</v>
       </c>
-      <c r="I64" t="n">
-        <v>31</v>
-      </c>
-      <c r="J64" t="n">
-        <v>232</v>
-      </c>
-      <c r="K64" t="n">
-        <v>-0.1142857142857143</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" t="n">
-        <v>22</v>
-      </c>
-      <c r="N64" t="n">
-        <v>-1</v>
+      <c r="O64" t="n">
+        <v>558</v>
       </c>
     </row>
     <row r="65">
@@ -4149,25 +4401,28 @@
         <v>-0.09999999999999998</v>
       </c>
       <c r="H65" t="n">
+        <v>17</v>
+      </c>
+      <c r="I65" t="n">
+        <v>249</v>
+      </c>
+      <c r="J65" t="n">
+        <v>-0.4516129032258065</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" t="n">
+        <v>22</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0</v>
+      </c>
+      <c r="N65" t="n">
         <v>4</v>
       </c>
-      <c r="I65" t="n">
-        <v>17</v>
-      </c>
-      <c r="J65" t="n">
-        <v>249</v>
-      </c>
-      <c r="K65" t="n">
-        <v>-0.4516129032258065</v>
-      </c>
-      <c r="L65" t="n">
-        <v>0</v>
-      </c>
-      <c r="M65" t="n">
-        <v>22</v>
-      </c>
-      <c r="N65" t="n">
-        <v>0</v>
+      <c r="O65" t="n">
+        <v>550</v>
       </c>
     </row>
     <row r="66">
@@ -4193,25 +4448,28 @@
         <v>-0.2222222222222222</v>
       </c>
       <c r="H66" t="n">
+        <v>22</v>
+      </c>
+      <c r="I66" t="n">
+        <v>271</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.2941176470588236</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" t="n">
+        <v>22</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" t="n">
         <v>2.892561983471075</v>
       </c>
-      <c r="I66" t="n">
-        <v>22</v>
-      </c>
-      <c r="J66" t="n">
-        <v>271</v>
-      </c>
-      <c r="K66" t="n">
-        <v>0.2941176470588236</v>
-      </c>
-      <c r="L66" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" t="n">
-        <v>22</v>
-      </c>
-      <c r="N66" t="n">
-        <v>0</v>
+      <c r="O66" t="n">
+        <v>535</v>
       </c>
     </row>
     <row r="67">
@@ -4237,25 +4495,28 @@
         <v>0</v>
       </c>
       <c r="H67" t="n">
+        <v>27</v>
+      </c>
+      <c r="I67" t="n">
+        <v>298</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.2272727272727273</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>22</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" t="n">
         <v>3.167420814479638</v>
       </c>
-      <c r="I67" t="n">
-        <v>27</v>
-      </c>
-      <c r="J67" t="n">
-        <v>298</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0.2272727272727273</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" t="n">
-        <v>22</v>
-      </c>
-      <c r="N67" t="n">
-        <v>0</v>
+      <c r="O67" t="n">
+        <v>515</v>
       </c>
     </row>
     <row r="68">
@@ -4281,25 +4542,28 @@
         <v>0.4285714285714286</v>
       </c>
       <c r="H68" t="n">
+        <v>38</v>
+      </c>
+      <c r="I68" t="n">
+        <v>336</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.4074074074074074</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>22</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" t="n">
         <v>4.347826086956522</v>
       </c>
-      <c r="I68" t="n">
-        <v>38</v>
-      </c>
-      <c r="J68" t="n">
-        <v>336</v>
-      </c>
-      <c r="K68" t="n">
-        <v>0.4074074074074074</v>
-      </c>
-      <c r="L68" t="n">
-        <v>0</v>
-      </c>
-      <c r="M68" t="n">
-        <v>22</v>
-      </c>
-      <c r="N68" t="n">
-        <v>0</v>
+      <c r="O68" t="n">
+        <v>487</v>
       </c>
     </row>
     <row r="69">
@@ -4325,25 +4589,28 @@
         <v>1.8</v>
       </c>
       <c r="H69" t="n">
+        <v>45</v>
+      </c>
+      <c r="I69" t="n">
+        <v>381</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.1842105263157894</v>
+      </c>
+      <c r="K69" t="n">
+        <v>3</v>
+      </c>
+      <c r="L69" t="n">
+        <v>25</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" t="n">
         <v>6.796116504854369</v>
       </c>
-      <c r="I69" t="n">
-        <v>45</v>
-      </c>
-      <c r="J69" t="n">
-        <v>381</v>
-      </c>
-      <c r="K69" t="n">
-        <v>0.1842105263157894</v>
-      </c>
-      <c r="L69" t="n">
-        <v>3</v>
-      </c>
-      <c r="M69" t="n">
-        <v>25</v>
-      </c>
-      <c r="N69" t="n">
-        <v>0</v>
+      <c r="O69" t="n">
+        <v>470</v>
       </c>
     </row>
     <row r="70">
@@ -4369,25 +4636,28 @@
         <v>-0.8571428571428572</v>
       </c>
       <c r="H70" t="n">
+        <v>22</v>
+      </c>
+      <c r="I70" t="n">
+        <v>403</v>
+      </c>
+      <c r="J70" t="n">
+        <v>-0.5111111111111111</v>
+      </c>
+      <c r="K70" t="n">
+        <v>1</v>
+      </c>
+      <c r="L70" t="n">
+        <v>26</v>
+      </c>
+      <c r="M70" t="n">
+        <v>-0.6666666666666667</v>
+      </c>
+      <c r="N70" t="n">
         <v>1.574803149606299</v>
       </c>
-      <c r="I70" t="n">
-        <v>22</v>
-      </c>
-      <c r="J70" t="n">
-        <v>403</v>
-      </c>
-      <c r="K70" t="n">
-        <v>-0.5111111111111111</v>
-      </c>
-      <c r="L70" t="n">
-        <v>1</v>
-      </c>
-      <c r="M70" t="n">
-        <v>26</v>
-      </c>
-      <c r="N70" t="n">
-        <v>-0.6666666666666667</v>
+      <c r="O70" t="n">
+        <v>452</v>
       </c>
     </row>
     <row r="71">
@@ -4413,25 +4683,28 @@
         <v>-0.75</v>
       </c>
       <c r="H71" t="n">
+        <v>87</v>
+      </c>
+      <c r="I71" t="n">
+        <v>490</v>
+      </c>
+      <c r="J71" t="n">
+        <v>2.954545454545455</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" t="n">
+        <v>26</v>
+      </c>
+      <c r="M71" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N71" t="n">
         <v>0.4545454545454545</v>
       </c>
-      <c r="I71" t="n">
-        <v>87</v>
-      </c>
-      <c r="J71" t="n">
-        <v>490</v>
-      </c>
-      <c r="K71" t="n">
-        <v>2.954545454545455</v>
-      </c>
-      <c r="L71" t="n">
-        <v>0</v>
-      </c>
-      <c r="M71" t="n">
-        <v>26</v>
-      </c>
-      <c r="N71" t="n">
-        <v>-1</v>
+      <c r="O71" t="n">
+        <v>366</v>
       </c>
     </row>
     <row r="72">
@@ -4457,25 +4730,28 @@
         <v>3</v>
       </c>
       <c r="H72" t="n">
+        <v>43</v>
+      </c>
+      <c r="I72" t="n">
+        <v>533</v>
+      </c>
+      <c r="J72" t="n">
+        <v>-0.5057471264367817</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" t="n">
+        <v>26</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" t="n">
         <v>1.234567901234568</v>
       </c>
-      <c r="I72" t="n">
-        <v>43</v>
-      </c>
-      <c r="J72" t="n">
-        <v>533</v>
-      </c>
-      <c r="K72" t="n">
-        <v>-0.5057471264367817</v>
-      </c>
-      <c r="L72" t="n">
-        <v>0</v>
-      </c>
-      <c r="M72" t="n">
-        <v>26</v>
-      </c>
-      <c r="N72" t="n">
-        <v>0</v>
+      <c r="O72" t="n">
+        <v>327</v>
       </c>
     </row>
     <row r="73">
@@ -4501,25 +4777,28 @@
         <v>-0.75</v>
       </c>
       <c r="H73" t="n">
+        <v>28</v>
+      </c>
+      <c r="I73" t="n">
+        <v>561</v>
+      </c>
+      <c r="J73" t="n">
+        <v>-0.3488372093023255</v>
+      </c>
+      <c r="K73" t="n">
+        <v>1</v>
+      </c>
+      <c r="L73" t="n">
+        <v>27</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" t="n">
         <v>0.4366812227074235</v>
       </c>
-      <c r="I73" t="n">
-        <v>28</v>
-      </c>
-      <c r="J73" t="n">
-        <v>561</v>
-      </c>
-      <c r="K73" t="n">
-        <v>-0.3488372093023255</v>
-      </c>
-      <c r="L73" t="n">
-        <v>1</v>
-      </c>
-      <c r="M73" t="n">
-        <v>27</v>
-      </c>
-      <c r="N73" t="n">
-        <v>0</v>
+      <c r="O73" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="74">
@@ -4545,25 +4824,28 @@
         <v>0</v>
       </c>
       <c r="H74" t="n">
+        <v>61</v>
+      </c>
+      <c r="I74" t="n">
+        <v>622</v>
+      </c>
+      <c r="J74" t="n">
+        <v>1.178571428571428</v>
+      </c>
+      <c r="K74" t="n">
+        <v>1</v>
+      </c>
+      <c r="L74" t="n">
+        <v>28</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="n">
         <v>0.411522633744856</v>
       </c>
-      <c r="I74" t="n">
-        <v>61</v>
-      </c>
-      <c r="J74" t="n">
-        <v>622</v>
-      </c>
-      <c r="K74" t="n">
-        <v>1.178571428571428</v>
-      </c>
-      <c r="L74" t="n">
-        <v>1</v>
-      </c>
-      <c r="M74" t="n">
-        <v>28</v>
-      </c>
-      <c r="N74" t="n">
-        <v>0</v>
+      <c r="O74" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="75">
@@ -4589,25 +4871,28 @@
         <v>7</v>
       </c>
       <c r="H75" t="n">
+        <v>31</v>
+      </c>
+      <c r="I75" t="n">
+        <v>653</v>
+      </c>
+      <c r="J75" t="n">
+        <v>-0.4918032786885246</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" t="n">
+        <v>28</v>
+      </c>
+      <c r="M75" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N75" t="n">
         <v>4.519774011299435</v>
       </c>
-      <c r="I75" t="n">
-        <v>31</v>
-      </c>
-      <c r="J75" t="n">
-        <v>653</v>
-      </c>
-      <c r="K75" t="n">
-        <v>-0.4918032786885246</v>
-      </c>
-      <c r="L75" t="n">
-        <v>0</v>
-      </c>
-      <c r="M75" t="n">
-        <v>28</v>
-      </c>
-      <c r="N75" t="n">
-        <v>-1</v>
+      <c r="O75" t="n">
+        <v>217</v>
       </c>
     </row>
     <row r="76">
@@ -4633,25 +4918,28 @@
         <v>0.75</v>
       </c>
       <c r="H76" t="n">
+        <v>2</v>
+      </c>
+      <c r="I76" t="n">
+        <v>655</v>
+      </c>
+      <c r="J76" t="n">
+        <v>-0.935483870967742</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L76" t="n">
+        <v>28</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N76" t="n">
         <v>7.000000000000001</v>
       </c>
-      <c r="I76" t="n">
-        <v>2</v>
-      </c>
-      <c r="J76" t="n">
-        <v>655</v>
-      </c>
-      <c r="K76" t="n">
-        <v>-0.935483870967742</v>
-      </c>
-      <c r="L76" t="n">
-        <v>0</v>
-      </c>
-      <c r="M76" t="n">
-        <v>28</v>
-      </c>
-      <c r="N76" t="n">
-        <v>0</v>
+      <c r="O76" t="n">
+        <v>229</v>
       </c>
     </row>
     <row r="77">
@@ -4677,25 +4965,28 @@
         <v>-0.2142857142857143</v>
       </c>
       <c r="H77" t="n">
+        <v>2</v>
+      </c>
+      <c r="I77" t="n">
+        <v>657</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" t="n">
+        <v>28</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
         <v>5.583756345177665</v>
       </c>
-      <c r="I77" t="n">
-        <v>2</v>
-      </c>
-      <c r="J77" t="n">
-        <v>657</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0</v>
-      </c>
-      <c r="L77" t="n">
-        <v>0</v>
-      </c>
-      <c r="M77" t="n">
-        <v>28</v>
-      </c>
-      <c r="N77" t="n">
-        <v>0</v>
+      <c r="O77" t="n">
+        <v>238</v>
       </c>
     </row>
     <row r="78">
@@ -4721,25 +5012,28 @@
         <v>1.181818181818182</v>
       </c>
       <c r="H78" t="n">
+        <v>14</v>
+      </c>
+      <c r="I78" t="n">
+        <v>671</v>
+      </c>
+      <c r="J78" t="n">
+        <v>6</v>
+      </c>
+      <c r="K78" t="n">
+        <v>1</v>
+      </c>
+      <c r="L78" t="n">
+        <v>29</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" t="n">
         <v>9.338521400778211</v>
       </c>
-      <c r="I78" t="n">
-        <v>14</v>
-      </c>
-      <c r="J78" t="n">
-        <v>671</v>
-      </c>
-      <c r="K78" t="n">
-        <v>6</v>
-      </c>
-      <c r="L78" t="n">
-        <v>1</v>
-      </c>
-      <c r="M78" t="n">
-        <v>29</v>
-      </c>
-      <c r="N78" t="n">
-        <v>0</v>
+      <c r="O78" t="n">
+        <v>248</v>
       </c>
     </row>
     <row r="79">
@@ -4765,25 +5059,28 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>671</v>
+      </c>
+      <c r="J79" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" t="n">
+        <v>29</v>
+      </c>
+      <c r="M79" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N79" t="n">
         <v>3.137254901960784</v>
       </c>
-      <c r="I79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" t="n">
-        <v>671</v>
-      </c>
-      <c r="K79" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L79" t="n">
-        <v>0</v>
-      </c>
-      <c r="M79" t="n">
-        <v>29</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-1</v>
+      <c r="O79" t="n">
+        <v>256</v>
       </c>
     </row>
     <row r="80">
@@ -4809,25 +5106,28 @@
         <v>1.25</v>
       </c>
       <c r="H80" t="n">
+        <v>19</v>
+      </c>
+      <c r="I80" t="n">
+        <v>690</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" t="n">
+        <v>29</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" t="n">
         <v>6</v>
       </c>
-      <c r="I80" t="n">
-        <v>19</v>
-      </c>
-      <c r="J80" t="n">
-        <v>690</v>
-      </c>
-      <c r="K80" t="n">
-        <v>0</v>
-      </c>
-      <c r="L80" t="n">
-        <v>0</v>
-      </c>
-      <c r="M80" t="n">
-        <v>29</v>
-      </c>
-      <c r="N80" t="n">
-        <v>0</v>
+      <c r="O80" t="n">
+        <v>255</v>
       </c>
     </row>
     <row r="81">
@@ -4853,25 +5153,28 @@
         <v>-0.4444444444444444</v>
       </c>
       <c r="H81" t="n">
+        <v>1</v>
+      </c>
+      <c r="I81" t="n">
+        <v>691</v>
+      </c>
+      <c r="J81" t="n">
+        <v>-0.9473684210526316</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" t="n">
+        <v>29</v>
+      </c>
+      <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" t="n">
         <v>4.23728813559322</v>
       </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="n">
-        <v>691</v>
-      </c>
-      <c r="K81" t="n">
-        <v>-0.9473684210526316</v>
-      </c>
-      <c r="L81" t="n">
-        <v>0</v>
-      </c>
-      <c r="M81" t="n">
-        <v>29</v>
-      </c>
-      <c r="N81" t="n">
-        <v>0</v>
+      <c r="O81" t="n">
+        <v>264</v>
       </c>
     </row>
     <row r="82">
@@ -4897,25 +5200,28 @@
         <v>1.3</v>
       </c>
       <c r="H82" t="n">
+        <v>22</v>
+      </c>
+      <c r="I82" t="n">
+        <v>713</v>
+      </c>
+      <c r="J82" t="n">
+        <v>21</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" t="n">
+        <v>29</v>
+      </c>
+      <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" t="n">
         <v>5.651105651105651</v>
       </c>
-      <c r="I82" t="n">
-        <v>22</v>
-      </c>
-      <c r="J82" t="n">
-        <v>713</v>
-      </c>
-      <c r="K82" t="n">
-        <v>21</v>
-      </c>
-      <c r="L82" t="n">
-        <v>0</v>
-      </c>
-      <c r="M82" t="n">
-        <v>29</v>
-      </c>
-      <c r="N82" t="n">
-        <v>0</v>
+      <c r="O82" t="n">
+        <v>265</v>
       </c>
     </row>
     <row r="83">
@@ -4941,25 +5247,28 @@
         <v>-0.6956521739130435</v>
       </c>
       <c r="H83" t="n">
+        <v>23</v>
+      </c>
+      <c r="I83" t="n">
+        <v>736</v>
+      </c>
+      <c r="J83" t="n">
+        <v>0.04545454545454541</v>
+      </c>
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
+      <c r="L83" t="n">
+        <v>29</v>
+      </c>
+      <c r="M83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" t="n">
         <v>3.465346534653466</v>
       </c>
-      <c r="I83" t="n">
-        <v>23</v>
-      </c>
-      <c r="J83" t="n">
-        <v>736</v>
-      </c>
-      <c r="K83" t="n">
-        <v>0.04545454545454541</v>
-      </c>
-      <c r="L83" t="n">
-        <v>0</v>
-      </c>
-      <c r="M83" t="n">
-        <v>29</v>
-      </c>
-      <c r="N83" t="n">
-        <v>0</v>
+      <c r="O83" t="n">
+        <v>249</v>
       </c>
     </row>
     <row r="84">
@@ -4985,25 +5294,28 @@
         <v>-0.5714285714285714</v>
       </c>
       <c r="H84" t="n">
+        <v>18</v>
+      </c>
+      <c r="I84" t="n">
+        <v>754</v>
+      </c>
+      <c r="J84" t="n">
+        <v>-0.2173913043478261</v>
+      </c>
+      <c r="K84" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" t="n">
+        <v>29</v>
+      </c>
+      <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" t="n">
         <v>1.5</v>
       </c>
-      <c r="I84" t="n">
-        <v>18</v>
-      </c>
-      <c r="J84" t="n">
-        <v>754</v>
-      </c>
-      <c r="K84" t="n">
-        <v>-0.2173913043478261</v>
-      </c>
-      <c r="L84" t="n">
-        <v>0</v>
-      </c>
-      <c r="M84" t="n">
-        <v>29</v>
-      </c>
-      <c r="N84" t="n">
-        <v>0</v>
+      <c r="O84" t="n">
+        <v>234</v>
       </c>
     </row>
     <row r="85">
@@ -5029,25 +5341,75 @@
         <v>-0.6666666666666667</v>
       </c>
       <c r="H85" t="n">
+        <v>15</v>
+      </c>
+      <c r="I85" t="n">
+        <v>769</v>
+      </c>
+      <c r="J85" t="n">
+        <v>-0.1666666666666666</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" t="n">
+        <v>29</v>
+      </c>
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" t="n">
         <v>0.4739336492890995</v>
       </c>
-      <c r="I85" t="n">
-        <v>15</v>
-      </c>
-      <c r="J85" t="n">
-        <v>769</v>
-      </c>
-      <c r="K85" t="n">
-        <v>-0.1666666666666666</v>
-      </c>
-      <c r="L85" t="n">
-        <v>0</v>
-      </c>
-      <c r="M85" t="n">
+      <c r="O85" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>43971</v>
+      </c>
+      <c r="B86" t="n">
+        <v>208</v>
+      </c>
+      <c r="C86" t="n">
+        <v>12405</v>
+      </c>
+      <c r="D86" t="n">
+        <v>-0.01421800947867302</v>
+      </c>
+      <c r="E86" t="n">
+        <v>14</v>
+      </c>
+      <c r="F86" t="n">
+        <v>1003</v>
+      </c>
+      <c r="G86" t="n">
+        <v>13</v>
+      </c>
+      <c r="H86" t="n">
+        <v>3</v>
+      </c>
+      <c r="I86" t="n">
+        <v>772</v>
+      </c>
+      <c r="J86" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="K86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" t="n">
         <v>29</v>
       </c>
-      <c r="N85" t="n">
-        <v>0</v>
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" t="n">
+        <v>6.730769230769231</v>
+      </c>
+      <c r="O86" t="n">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>